<commit_message>
Newest push to website
</commit_message>
<xml_diff>
--- a/CodeSystem-cbs-temp-code-system.xlsx
+++ b/CodeSystem-cbs-temp-code-system.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2021-11-03T10:06:32-04:00</t>
+    <t>2022-01-18T12:41:26-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -318,10 +318,10 @@
     <t>History of Encounters (Hospitalizations)</t>
   </si>
   <si>
-    <t>epi-questions</t>
-  </si>
-  <si>
-    <t>Epi Questionnaires and Observations</t>
+    <t>epi-observations</t>
+  </si>
+  <si>
+    <t>Epi Observations</t>
   </si>
   <si>
     <t>occupational-data</t>

</xml_diff>

<commit_message>
v0.2.0 version of the CBS IG
</commit_message>
<xml_diff>
--- a/CodeSystem-cbs-temp-code-system.xlsx
+++ b/CodeSystem-cbs-temp-code-system.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="122">
   <si>
     <t>Property</t>
   </si>
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.0</t>
+    <t>0.2.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-01-25T10:18:17-05:00</t>
+    <t>2022-02-08T17:12:45-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -87,6 +87,9 @@
     <t>Case Sensitive</t>
   </si>
   <si>
+    <t>true</t>
+  </si>
+  <si>
     <t>Value Set (all codes)</t>
   </si>
   <si>
@@ -111,7 +114,7 @@
     <t>Count</t>
   </si>
   <si>
-    <t>35</t>
+    <t>36</t>
   </si>
   <si>
     <t>Level</t>
@@ -370,6 +373,12 @@
   </si>
   <si>
     <t>Vital Records Reporting (Death, Birth, or Fetal Death)</t>
+  </si>
+  <si>
+    <t>lab-interpretative-report</t>
+  </si>
+  <si>
+    <t>Lab Interpretive Report</t>
   </si>
 </sst>
 </file>
@@ -615,52 +624,54 @@
       <c r="A14" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" t="s" s="2">
+        <v>24</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B15" s="2"/>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" s="2"/>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B20" s="2"/>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -670,7 +681,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -678,459 +689,471 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s" s="1">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s" s="1">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D1" t="s" s="1">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C6" t="s" s="2">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D6" t="s" s="2">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C7" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D7" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C8" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D8" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C9" t="s" s="2">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D9" t="s" s="2">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C10" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D10" t="s" s="2">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C11" t="s" s="2">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D11" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C12" t="s" s="2">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D12" t="s" s="2">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C13" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C14" t="s" s="2">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D14" s="2"/>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C15" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D15" s="2"/>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C16" t="s" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C17" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D17" s="2"/>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C18" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C19" t="s" s="2">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D19" s="2"/>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C20" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D20" s="2"/>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C21" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D21" s="2"/>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C22" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D22" s="2"/>
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C23" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D23" s="2"/>
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C24" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D24" s="2"/>
     </row>
     <row r="25">
       <c r="A25" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C25" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D25" s="2"/>
     </row>
     <row r="26">
       <c r="A26" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C26" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D26" s="2"/>
     </row>
     <row r="27">
       <c r="A27" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C27" t="s" s="2">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D27" s="2"/>
     </row>
     <row r="28">
       <c r="A28" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C28" t="s" s="2">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D28" s="2"/>
     </row>
     <row r="29">
       <c r="A29" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C29" t="s" s="2">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D29" s="2"/>
     </row>
     <row r="30">
       <c r="A30" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C30" t="s" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D30" s="2"/>
     </row>
     <row r="31">
       <c r="A31" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C31" t="s" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D31" s="2"/>
     </row>
     <row r="32">
       <c r="A32" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C32" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D32" s="2"/>
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C33" t="s" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D33" s="2"/>
     </row>
     <row r="34">
       <c r="A34" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C34" t="s" s="2">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D34" s="2"/>
     </row>
     <row r="35">
       <c r="A35" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C35" t="s" s="2">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D35" s="2"/>
     </row>
     <row r="36">
       <c r="A36" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C36" t="s" s="2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D36" s="2"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="B37" t="s" s="2">
+        <v>120</v>
+      </c>
+      <c r="C37" t="s" s="2">
+        <v>121</v>
+      </c>
+      <c r="D37" s="2"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
Pushing v0.2.1 release to website
</commit_message>
<xml_diff>
--- a/CodeSystem-cbs-temp-code-system.xlsx
+++ b/CodeSystem-cbs-temp-code-system.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.2.0</t>
+    <t>0.2.1</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-02-08T17:12:45-05:00</t>
+    <t>2022-02-17T15:59:55-05:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>